<commit_message>
updated members and payment spreadsheets
</commit_message>
<xml_diff>
--- a/core/management/commands/GCCWELFARE DATABASE.xlsx
+++ b/core/management/commands/GCCWELFARE DATABASE.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1659" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1659" uniqueCount="1082">
   <si>
     <t xml:space="preserve">Salutation</t>
   </si>
@@ -3266,10 +3266,7 @@
     <t xml:space="preserve">7219-00300-Nairobi</t>
   </si>
   <si>
-    <t xml:space="preserve">TERESIAH NYOKABI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7220-00300-Nairobi</t>
+    <t xml:space="preserve">JACKLINE KARANJA</t>
   </si>
 </sst>
 </file>
@@ -3279,7 +3276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3301,6 +3298,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3345,12 +3348,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3371,10 +3378,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y189"/>
+  <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A173" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I189" activeCellId="0" sqref="I189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10240,35 +10247,37 @@
         <v>20744551</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B189" s="0" t="s">
+      <c r="B189" s="2" t="s">
         <v>1081</v>
       </c>
       <c r="C189" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D189" s="0" t="n">
+      <c r="D189" s="2" t="n">
         <v>99744600</v>
       </c>
-      <c r="E189" s="0" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F189" s="0" t="n">
+      <c r="E189" s="2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F189" s="2" t="n">
+        <v>715130036</v>
+      </c>
+      <c r="G189" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H189" s="2" t="n">
         <v>20744551</v>
       </c>
-      <c r="G189" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="H189" s="0" t="n">
-        <v>20744551</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="pmnyagah@gmail.com"/>
+    <hyperlink ref="G189" r:id="rId2" display="xyz@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
update faith N MBUTHIA payment details - incorrect last_name
</commit_message>
<xml_diff>
--- a/core/management/commands/GCCWELFARE DATABASE.xlsx
+++ b/core/management/commands/GCCWELFARE DATABASE.xlsx
@@ -3276,7 +3276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3298,12 +3298,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3348,16 +3342,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3380,8 +3370,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A173" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I189" activeCellId="0" sqref="I189"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A126" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B138" activeCellId="0" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10251,25 +10241,25 @@
       <c r="A189" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="B189" s="1" t="s">
         <v>1081</v>
       </c>
       <c r="C189" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D189" s="2" t="n">
+      <c r="D189" s="1" t="n">
         <v>99744600</v>
       </c>
-      <c r="E189" s="2" t="s">
+      <c r="E189" s="1" t="s">
         <v>1080</v>
       </c>
-      <c r="F189" s="2" t="n">
+      <c r="F189" s="1" t="n">
         <v>715130036</v>
       </c>
-      <c r="G189" s="2" t="s">
+      <c r="G189" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H189" s="2" t="n">
+      <c r="H189" s="1" t="n">
         <v>20744551</v>
       </c>
     </row>

</xml_diff>